<commit_message>
update mdl, mpcbs, raf
</commit_message>
<xml_diff>
--- a/InputData/elec/RAF/Regional Availability Factor.xlsx
+++ b/InputData/elec/RAF/Regional Availability Factor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\RMI\RMI_all_states\MT\elec\RAF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5563100B-23AF-4325-B65D-F8A3D276A75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AF73543-D6F1-4EAA-8733-34025A4F78A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11145" yWindow="825" windowWidth="16755" windowHeight="16170" activeTab="1" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
+    <workbookView xWindow="1725" yWindow="1725" windowWidth="14400" windowHeight="7290" firstSheet="2" activeTab="3" xr2:uid="{D718C537-5235-45E1-A117-07B097D2BDF0}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -621,9 +621,9 @@
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -631,20 +631,20 @@
         <v>67</v>
       </c>
       <c r="C1" s="3">
-        <v>45366</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45376</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,167 +652,167 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A34" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A35" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A36" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A38" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A39" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A40" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A41" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A42" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A43" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A45" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A46" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A47" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A48" t="s">
         <v>66</v>
       </c>
@@ -830,16 +830,16 @@
   </sheetPr>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -847,7 +847,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -855,7 +855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -863,7 +863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -871,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -879,7 +879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -887,7 +887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -895,7 +895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -903,7 +903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -911,7 +911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -919,7 +919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -927,7 +927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -935,7 +935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -943,7 +943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -951,7 +951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -959,7 +959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -967,7 +967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -975,7 +975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -983,7 +983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -991,7 +991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -999,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1055,13 +1055,13 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="34.54296875" customWidth="1"/>
+    <col min="2" max="2" width="19.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1089,13 +1089,16 @@
   </sheetPr>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="29.04296875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1103,7 +1106,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1111,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1119,7 +1122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1127,7 +1130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1135,7 +1138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1143,7 +1146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1159,7 +1162,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1167,7 +1170,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1175,7 +1178,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1183,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1191,7 +1194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1199,7 +1202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1207,7 +1210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1215,7 +1218,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1223,7 +1226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1231,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1239,7 +1242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1247,7 +1250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1255,7 +1258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1263,7 +1266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1271,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1279,20 +1282,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>47</v>
       </c>
       <c r="B24">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>48</v>
       </c>
       <c r="B25">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>